<commit_message>
parse multiple files - bit of a refactoring needed with the test
</commit_message>
<xml_diff>
--- a/tests/resources/test_template2.xlsx
+++ b/tests/resources/test_template2.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="6">
   <si>
     <t xml:space="preserve">Date:</t>
   </si>
@@ -37,6 +37,9 @@
   <si>
     <t xml:space="preserve">Integer:</t>
   </si>
+  <si>
+    <t xml:space="preserve">MEGA VALUE</t>
+  </si>
 </sst>
 </file>
 
@@ -51,6 +54,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -136,10 +140,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:B5"/>
+  <dimension ref="A2:C5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -177,6 +181,9 @@
       </c>
       <c r="B5" s="0" t="n">
         <v>10</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1837,7 +1844,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>